<commit_message>
mais vagas, beneficios, nome do arquivo
</commit_message>
<xml_diff>
--- a/job_info_gpt3.xlsx
+++ b/job_info_gpt3.xlsx
@@ -425,7 +425,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:H48"/>
+  <dimension ref="A1:I48"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -461,15 +461,20 @@
       </c>
       <c r="F1" s="1" t="inlineStr">
         <is>
+          <t>Carga Horária</t>
+        </is>
+      </c>
+      <c r="G1" s="1" t="inlineStr">
+        <is>
           <t>Destinatários</t>
         </is>
       </c>
-      <c r="G1" s="1" t="inlineStr">
+      <c r="H1" s="1" t="inlineStr">
         <is>
           <t>Áreas de Atuação</t>
         </is>
       </c>
-      <c r="H1" s="1" t="inlineStr">
+      <c r="I1" s="1" t="inlineStr">
         <is>
           <t>Responsabilidades</t>
         </is>
@@ -498,22 +503,27 @@
       </c>
       <c r="E2" t="inlineStr">
         <is>
-          <t>R$ 3.900,00 (R$ 3000,00 contrato de estágio + R$ 900,00 em benefícios)</t>
+          <t>R$ 3.900,00</t>
         </is>
       </c>
       <c r="F2" t="inlineStr">
         <is>
-          <t>Jovens brilhantes e ambiciosos</t>
+          <t>100% remota</t>
         </is>
       </c>
       <c r="G2" t="inlineStr">
         <is>
+          <t>Jovens</t>
+        </is>
+      </c>
+      <c r="H2" t="inlineStr">
+        <is>
           <t>Engenharia de Software</t>
         </is>
       </c>
-      <c r="H2" t="inlineStr">
-        <is>
-          <t>Adquirir conhecimento em tecnologias modernas, desenvolver produtos de software, influenciar o desenvolvimento de produto.</t>
+      <c r="I2" t="inlineStr">
+        <is>
+          <t>Desenvolver produtos de software, adquirir conhecimento em tecnologias modernas.</t>
         </is>
       </c>
     </row>
@@ -525,7 +535,7 @@
       </c>
       <c r="B3" t="inlineStr">
         <is>
-          <t>Desenvolvedor BackEnd Java/Kotlin Especialista II (Engenharia de Crédito)</t>
+          <t>Pessoa Desenvolvedora BackEnd Java/Kotlin Especialista II (Engenharia de Crédito) (Produtos Digitais Financeiros)</t>
         </is>
       </c>
       <c r="C3" t="inlineStr">
@@ -535,7 +545,7 @@
       </c>
       <c r="D3" t="inlineStr">
         <is>
-          <t>Experiência relevante, habilidades técnicas, liderança, resolução de problemas, comunicação, conhecimento em AWS, Python, JavaScript/TypeScript, Java/Kotlin, estruturas de dados, monitoração e logging, Rest, orientação a eventos, testes unitários e de integração, CI/CD, serverless framework, times ágeis, banco de dados, produtos financeiros, testes de carga.</t>
+          <t>Experiência relevante, habilidades técnicas avançadas, liderança, resolução de problemas, comunicação, mentalidade orientada a resultados, conhecimento em AWS, Python, JavaScript/TypeScript, Java/Kotlin, estruturas de dados, monitoração, Rest, orientação a eventos, testes unitários, CI/CD, serverless framework, times ágeis, banco de dados, produtos financeiros, entre outros.</t>
         </is>
       </c>
       <c r="E3" t="inlineStr">
@@ -545,17 +555,22 @@
       </c>
       <c r="F3" t="inlineStr">
         <is>
+          <t>Flexível e sustentável</t>
+        </is>
+      </c>
+      <c r="G3" t="inlineStr">
+        <is>
           <t>Pessoas com deficiência, pessoas negras, mulheres, LGBTQIA+, pessoas 50+</t>
         </is>
       </c>
-      <c r="G3" t="inlineStr">
-        <is>
-          <t>Engenharia de Crédito</t>
-        </is>
-      </c>
       <c r="H3" t="inlineStr">
         <is>
-          <t>Desenvolvimento de soluções em nuvem, liderança técnica, arquitetura escalável e segura na AWS, participação no desenho da arquitetura de solução, desenvolvimento de código de alta qualidade, manutenção de base de código, resolução de problemas técnicos, atualização sobre tecnologias, colaboração com equipes multifuncionais, orientação técnica, suporte à equipe, evolução técnica dos desenvolvedores.</t>
+          <t>Desenvolvimento de Plataforma de Crédito, Produtos Digitais Financeiros</t>
+        </is>
+      </c>
+      <c r="I3" t="inlineStr">
+        <is>
+          <t>Desenvolvimento de soluções em nuvem, liderança técnica, participação no desenho da arquitetura, desenvolvimento de código de alta qualidade, investigação e resolução de problemas técnicos, atualização sobre tendências tecnológicas, colaboração com equipes multifuncionais, entre outros.</t>
         </is>
       </c>
     </row>
@@ -577,7 +592,7 @@
       </c>
       <c r="D4" t="inlineStr">
         <is>
-          <t>Comunicação interpessoal, matrícula ativa em curso superior, conhecimentos em ferramentas de Analytics, inglês para leitura</t>
+          <t>Comunicação interpessoal, interesse em aprender, curso superior ativo</t>
         </is>
       </c>
       <c r="E4" t="inlineStr">
@@ -587,17 +602,22 @@
       </c>
       <c r="F4" t="inlineStr">
         <is>
-          <t>Estudantes universitários</t>
+          <t>Não especificada</t>
         </is>
       </c>
       <c r="G4" t="inlineStr">
         <is>
+          <t>Estudantes de tecnologia, administração, publicidade, marketing, engenharias ou áreas correlatas</t>
+        </is>
+      </c>
+      <c r="H4" t="inlineStr">
+        <is>
           <t>Data &amp; Analytics</t>
         </is>
       </c>
-      <c r="H4" t="inlineStr">
-        <is>
-          <t>Participar de reuniões, implementar e gerir tags e plataformas de Digital Analytics, criar e manter bases de dados, planejar métricas, auxiliar na confecção de dashboards e relatórios.</t>
+      <c r="I4" t="inlineStr">
+        <is>
+          <t>Participar de reuniões, implementar e gerir tags de Digital Analytics, criar e manter bases de dados, planejar métricas, auxiliar na confecção de dashboards e relatórios.</t>
         </is>
       </c>
     </row>
@@ -619,7 +639,7 @@
       </c>
       <c r="D5" t="inlineStr">
         <is>
-          <t>Estudante, 2° semestre, disponibilidade, curioso</t>
+          <t>Estudante, 2° semestre, curioso, questionador</t>
         </is>
       </c>
       <c r="E5" t="inlineStr">
@@ -629,17 +649,22 @@
       </c>
       <c r="F5" t="inlineStr">
         <is>
+          <t>4h ou 6h diárias</t>
+        </is>
+      </c>
+      <c r="G5" t="inlineStr">
+        <is>
           <t>Estudantes de graduação ou tecnólogo</t>
         </is>
       </c>
-      <c r="G5" t="inlineStr">
-        <is>
-          <t>Tecnologia, Comunicação, Riscos, Jurídico, Atacado</t>
-        </is>
-      </c>
       <c r="H5" t="inlineStr">
         <is>
-          <t>Desenvolver potencial, participar de projetos, aprender com liderança</t>
+          <t>Diversas áreas do banco (Tecnologia, Comunicação, Riscos, Jurídico, Atacado)</t>
+        </is>
+      </c>
+      <c r="I5" t="inlineStr">
+        <is>
+          <t>Participar de projetos importantes para o banco, aprender com a liderança, interagir em equipe.</t>
         </is>
       </c>
     </row>
@@ -661,7 +686,7 @@
       </c>
       <c r="D6" t="inlineStr">
         <is>
-          <t>Cursando ensino superior em áreas correlatas, conhecimento em Java, Spring Boot, Hibernate/JPA, bancos de dados, capacidade de trabalho em equipe e boa comunicação</t>
+          <t>Cursando ensino superior em Ciência da Computação, Engenharia de Software, Sistemas de Informação ou áreas correlatas, conhecimento em Orientação a Objetos, Java 8+, Spring Boot, Hibernate/JPA, bancos de dados relacionais e NoSQL, capacidade de atuar em equipe e boa comunicação.</t>
         </is>
       </c>
       <c r="E6" t="inlineStr">
@@ -671,17 +696,22 @@
       </c>
       <c r="F6" t="inlineStr">
         <is>
-          <t>Estudantes de Ciência da Computação, Engenharia de Software, Sistemas de Informação, etc.</t>
+          <t>Não especificada</t>
         </is>
       </c>
       <c r="G6" t="inlineStr">
         <is>
-          <t>Desenvolvimento de aplicações Java em microsserviços</t>
+          <t>Estudantes de áreas relacionadas à tecnologia</t>
         </is>
       </c>
       <c r="H6" t="inlineStr">
         <is>
-          <t>Desenvolvimento supervisionado, colaboração em fases do ciclo de vida do software, documentação técnica, resolução de problemas, trabalho com metodologia ágil Scrum.</t>
+          <t>Desenvolvimento Backend</t>
+        </is>
+      </c>
+      <c r="I6" t="inlineStr">
+        <is>
+          <t>Desenvolver aplicações Java, colaborar com a equipe de desenvolvimento, documentar sistemas e aplicações, resolver problemas das aplicações, trabalhar com metodologia ágil Scrum.</t>
         </is>
       </c>
     </row>
@@ -698,7 +728,7 @@
       </c>
       <c r="C7" t="inlineStr">
         <is>
-          <t>Remoto, com presença mensal na Honda São Paulo</t>
+          <t>Remoto, São Paulo (próximo ao shopping Morumbi)</t>
         </is>
       </c>
       <c r="D7" t="inlineStr">
@@ -713,17 +743,22 @@
       </c>
       <c r="F7" t="inlineStr">
         <is>
-          <t>Estudantes de tecnologia da informação</t>
+          <t>Modelo virtual de trabalho, presencial na Honda Morumbi 1x por mês</t>
         </is>
       </c>
       <c r="G7" t="inlineStr">
         <is>
-          <t>Desenvolvimento de software e sistemas</t>
+          <t>Estudantes de graduação em tecnologia da informação</t>
         </is>
       </c>
       <c r="H7" t="inlineStr">
         <is>
-          <t>Apoio na entrega de produtos de software, aplicação de melhorias de codificação, gestão de fornecedores externos</t>
+          <t>Desenvolvimento de software e projetos de sistemas</t>
+        </is>
+      </c>
+      <c r="I7" t="inlineStr">
+        <is>
+          <t>Organização da entrega contínua de produtos de software, aplicação de melhorias práticas e técnicas de codificação, gestão de fornecedores externos.</t>
         </is>
       </c>
     </row>
@@ -745,7 +780,7 @@
       </c>
       <c r="D8" t="inlineStr">
         <is>
-          <t>Cursando graduação em Ciência da Computação, Engenharia de Software, Sistemas de Informação ou áreas afins, conhecimento em Python e JavaScript, interesse em aprender sobre MongoDB, boa comunicação e habilidades interpessoais</t>
+          <t>Cursando graduação em Ciência da Computação, Engenharia de Software, Sistemas de Informação ou áreas afins, conhecimento em Python e JavaScript, familiaridade com React.js, interesse em aprender sobre MongoDB, boa comunicação e habilidades interpessoais</t>
         </is>
       </c>
       <c r="E8" t="inlineStr">
@@ -755,17 +790,22 @@
       </c>
       <c r="F8" t="inlineStr">
         <is>
-          <t>Estudantes universitários</t>
+          <t>Estágio 30h</t>
         </is>
       </c>
       <c r="G8" t="inlineStr">
         <is>
+          <t>Estagiários</t>
+        </is>
+      </c>
+      <c r="H8" t="inlineStr">
+        <is>
           <t>Desenvolvimento de Software</t>
         </is>
       </c>
-      <c r="H8" t="inlineStr">
-        <is>
-          <t>Auxiliar no desenvolvimento e manutenção de infraestrutura backend, suportar implementação e gerenciamento de bancos de dados, participar do desenvolvimento de interfaces de usuário, colaborar com a equipe de desenvolvimento, participar de reuniões e sessões de brainstorming, manter a documentação técnica organizada e atualizada.</t>
+      <c r="I8" t="inlineStr">
+        <is>
+          <t>Desenvolvimento e manutenção de infraestrutura backend, suporte a bancos de dados MongoDB, desenvolvimento de interfaces de usuário, colaboração em equipe, participação em reuniões e brainstorming, organização da documentação técnica.</t>
         </is>
       </c>
     </row>
@@ -777,7 +817,7 @@
       </c>
       <c r="B9" t="inlineStr">
         <is>
-          <t>Programa de Estágio 2024</t>
+          <t>Estágio 2024 Atacado</t>
         </is>
       </c>
       <c r="C9" t="inlineStr">
@@ -787,7 +827,7 @@
       </c>
       <c r="D9" t="inlineStr">
         <is>
-          <t>Estudante de nível superior, disponibilidade de horas semanais, inglês intermediário</t>
+          <t>Estudante de nível superior cursando a partir do 2º semestre, disponibilidade de 20, 25 ou 30 horas semanais, inglês intermediário.</t>
         </is>
       </c>
       <c r="E9" t="inlineStr">
@@ -797,17 +837,22 @@
       </c>
       <c r="F9" t="inlineStr">
         <is>
+          <t>20, 25 ou 30 horas semanais</t>
+        </is>
+      </c>
+      <c r="G9" t="inlineStr">
+        <is>
           <t>Estudantes de nível superior</t>
         </is>
       </c>
-      <c r="G9" t="inlineStr">
+      <c r="H9" t="inlineStr">
         <is>
           <t>Atacado</t>
         </is>
       </c>
-      <c r="H9" t="inlineStr">
-        <is>
-          <t>Desenvolver-se em diversas áreas, atender investidores, oferecer soluções financeiras.</t>
+      <c r="I9" t="inlineStr">
+        <is>
+          <t>Participar do propósito do Bradesco, atender investidores institucionais e clientes private banking.</t>
         </is>
       </c>
     </row>
@@ -839,17 +884,22 @@
       </c>
       <c r="F10" t="inlineStr">
         <is>
-          <t>Estudantes dos cursos mencionados</t>
+          <t>não especificada</t>
         </is>
       </c>
       <c r="G10" t="inlineStr">
         <is>
-          <t>Comércio Exterior, Logística</t>
+          <t>Estudantes universitários</t>
         </is>
       </c>
       <c r="H10" t="inlineStr">
         <is>
-          <t>Acompanhamento do fluxo de exportação, preparação de documentos, acompanhamento de coletas, responsável pelo fluxo de pagamentos dos fornecedores.</t>
+          <t>Comércio Exterior, Logística, Administração</t>
+        </is>
+      </c>
+      <c r="I10" t="inlineStr">
+        <is>
+          <t>Acompanhamento do fluxo de exportação, preparação de documentos, acompanhamento de coletas, responsável pelo fluxo de pagamentos.</t>
         </is>
       </c>
     </row>
@@ -871,7 +921,7 @@
       </c>
       <c r="D11" t="inlineStr">
         <is>
-          <t>Graduação em andamento, habilidades de planejamento de comunicação, experiência em redes sociais</t>
+          <t>Graduação em andamento, habilidades de comunicação, experiência em redes sociais</t>
         </is>
       </c>
       <c r="E11" t="inlineStr">
@@ -881,17 +931,22 @@
       </c>
       <c r="F11" t="inlineStr">
         <is>
-          <t>Estagiários em cursos correlatos a Publicação, Marketing ou Relações Públicas</t>
+          <t>Não especificada</t>
         </is>
       </c>
       <c r="G11" t="inlineStr">
         <is>
-          <t>Marketing</t>
+          <t>Estudantes de graduação em cursos correlatos a Publicidade, Marketing ou Relações Públicas</t>
         </is>
       </c>
       <c r="H11" t="inlineStr">
         <is>
-          <t>Auxiliar na concepção e entrega de estratégias de mídia social, criar planejamento de postagens, gerenciar campanhas, analisar desempenho em plataformas de mídia social, entre outras.</t>
+          <t>Marketing, Branding, Mídias Sociais</t>
+        </is>
+      </c>
+      <c r="I11" t="inlineStr">
+        <is>
+          <t>Auxiliar na criação de estratégias de mídias sociais, criar conteúdo, gerenciar campanhas, analisar desempenho, identificar tendências, otimizar interação.</t>
         </is>
       </c>
     </row>
@@ -913,7 +968,7 @@
       </c>
       <c r="D12" t="inlineStr">
         <is>
-          <t>Cursando graduação em Administração, Economia, Engenharia ou áreas relacionadas (a partir do 3º semestre), interesse por empreendedorismo, inovação e novas tecnologias, conhecimento em estratégia empresarial, pesquisa de mercado e análise de dados será um diferencial</t>
+          <t>Cursando graduação em Administração, Economia, Engenharia ou áreas relacionadas (a partir do 3º semestre), interesse por empreendedorismo, inovação e novas tecnologias, conhecimento em estratégia empresarial, pesquisa de mercado e análise de dados será um diferencial, habilidades analíticas, proatividade, autonomia, excelente comunicação oral e escrita.</t>
         </is>
       </c>
       <c r="E12" t="inlineStr">
@@ -923,17 +978,22 @@
       </c>
       <c r="F12" t="inlineStr">
         <is>
-          <t>Candidaturas diversas, incentivando a diversidade e inclusão</t>
+          <t>Não especificada</t>
         </is>
       </c>
       <c r="G12" t="inlineStr">
         <is>
-          <t>Estratégia Corporativa, Pesquisa de Mercado, Construção de Apresentações, Análise de Empresas, Suporte em Projetos de Consultoria</t>
+          <t>Estudantes de graduação</t>
         </is>
       </c>
       <c r="H12" t="inlineStr">
         <is>
-          <t>Auxiliar na formulação e implementação de estratégias corporativas, conduzir pesquisas de mercado, elaborar apresentações executivas, organizar e gerenciar informações do projeto, realizar análises financeiras e estratégicas de empresas, participar ativamente de projetos de consultoria.</t>
+          <t>Consultoria, Estratégia, Inteligência, Inovação</t>
+        </is>
+      </c>
+      <c r="I12" t="inlineStr">
+        <is>
+          <t>Auxiliar na formulação e implementação de estratégias corporativas, conduzir pesquisas de mercado, elaborar apresentações executivas, gestão de informações do projeto, análise financeira e estratégica de empresas, suporte em projetos de consultoria.</t>
         </is>
       </c>
     </row>
@@ -955,7 +1015,7 @@
       </c>
       <c r="D13" t="inlineStr">
         <is>
-          <t>Cursando ensino superior, computador com internet, disponibilidade mínima de 2 meses, conhecimento em lógica de programação</t>
+          <t>Cursando formação superior, computador com internet, disponibilidade mínima de 2 meses, conhecimento em lógica de programação</t>
         </is>
       </c>
       <c r="E13" t="inlineStr">
@@ -965,17 +1025,22 @@
       </c>
       <c r="F13" t="inlineStr">
         <is>
-          <t>Estudantes de ensino superior</t>
+          <t>Não especificada</t>
         </is>
       </c>
       <c r="G13" t="inlineStr">
         <is>
-          <t>Automation</t>
+          <t>Estudantes de formação superior</t>
         </is>
       </c>
       <c r="H13" t="inlineStr">
         <is>
-          <t>Desenvolver automações, construir telas, programar em Python, criar processos padronizados, lidar com produtos financeiros, prestar suporte, negociar prioridades, fomentar mudanças, documentar processos, desenvolver soluções, garantir estabilidade.</t>
+          <t>Automation, Discovery, Dev Team</t>
+        </is>
+      </c>
+      <c r="I13" t="inlineStr">
+        <is>
+          <t>Desenvolver automações, construir telas, programar em Python, criar processos padronizados, lidar com produtos financeiros, prestar suporte, negociar prioridades, documentar processos, acompanhar mapeamento de processos, desenvolver soluções de alto impacto, garantir estabilidade das soluções.</t>
         </is>
       </c>
     </row>
@@ -1005,19 +1070,20 @@
           <t>A combinar</t>
         </is>
       </c>
-      <c r="F14" t="inlineStr">
-        <is>
-          <t>Estudantes de áreas relacionadas</t>
-        </is>
-      </c>
+      <c r="F14" t="inlineStr"/>
       <c r="G14" t="inlineStr">
         <is>
-          <t>Marketing, Engenharia, Administração, Data Science</t>
+          <t>Estudantes universitários</t>
         </is>
       </c>
       <c r="H14" t="inlineStr">
         <is>
-          <t>Planejamento, implementação e análise de desempenho de comunicações, criação de conteúdo, desenvolvimento de relatórios, contribuição para geração de demanda e métricas de CRM.</t>
+          <t>Marketing, engenharia, administração, data science</t>
+        </is>
+      </c>
+      <c r="I14" t="inlineStr">
+        <is>
+          <t>Planejamento, implementação e análise de desempenho de comunicações, criação de conteúdo, desenvolvimento de relatórios, contribuição para geração de demanda e melhoria de métricas de CRM.</t>
         </is>
       </c>
     </row>
@@ -1029,12 +1095,12 @@
       </c>
       <c r="B15" t="inlineStr">
         <is>
-          <t>Estágio Engenheiro(a) de Dados</t>
+          <t>Engenheiro(a) de Dados</t>
         </is>
       </c>
       <c r="C15" t="inlineStr">
         <is>
-          <t>Remoto / Híbrido</t>
+          <t>Remoto</t>
         </is>
       </c>
       <c r="D15" t="inlineStr">
@@ -1049,17 +1115,22 @@
       </c>
       <c r="F15" t="inlineStr">
         <is>
+          <t>Não especificado</t>
+        </is>
+      </c>
+      <c r="G15" t="inlineStr">
+        <is>
           <t>Pessoas em graduação</t>
         </is>
       </c>
-      <c r="G15" t="inlineStr">
+      <c r="H15" t="inlineStr">
         <is>
           <t>Engenharia de Dados</t>
         </is>
       </c>
-      <c r="H15" t="inlineStr">
-        <is>
-          <t>Modelagem, coleta, limpeza e transformação de dados, suporte na construção de pipelines, participação na modelagem de dados para soluções de GenAI, colaboração com equipes multidisciplinares, criação e otimização de bancos de dados, apoio na definição e implementação de arquitetura de dados, implementação de políticas de governança de dados, contribuição na documentação dos processos e fluxos de dados.</t>
+      <c r="I15" t="inlineStr">
+        <is>
+          <t>Modelagem, coleta, limpeza e transformação de dados, suporte na construção e manutenção de pipelines de dados, colaboração com equipes multidisciplinares, participação na criação e otimização de bancos de dados, entre outras.</t>
         </is>
       </c>
     </row>
@@ -1081,27 +1152,32 @@
       </c>
       <c r="D16" t="inlineStr">
         <is>
-          <t>Disponibilidade 30h semanais, formatura até Dezembro/2025, curso relacionado a ciência, tecnologia, engenharia, matemática ou marketing, conhecimento básico de Google Ads e Facebook Ads, inglês intermediário, habilidade analítica, habilidade em equipe, capacidade de comunicação, certificações e projetos de mídias de performance são diferenciais.</t>
+          <t>Disponibilidade 30 horas semanais, formatura até Dezembro/2025, curso superior em ciência, tecnologia, engenharia, matemática ou marketing, conhecimento básico em Google Ads e Facebook Ads, inglês intermediário, habilidade em solucionar problemas de forma analítica e quantitativa, habilidade de trabalho em equipe, capacidade de comunicação, certificações em Google Ads, Facebook Ads e Bing Ads, projetos de mídias de performance, habilidade com planilhas e boas práticas de Copywriting</t>
         </is>
       </c>
       <c r="E16" t="inlineStr">
         <is>
-          <t>Salário a combinar</t>
+          <t>A combinar</t>
         </is>
       </c>
       <c r="F16" t="inlineStr">
         <is>
-          <t>Estudantes universitários</t>
+          <t>Pelo menos 30 horas semanais</t>
         </is>
       </c>
       <c r="G16" t="inlineStr">
         <is>
-          <t>Marketing, tecnologia, dados</t>
+          <t>Estudantes com previsão de formatura até Dezembro/2025</t>
         </is>
       </c>
       <c r="H16" t="inlineStr">
         <is>
-          <t>Gestão de mídias pagas, análise de resultados, planejamento de investimentos, gerenciamento de operações, contribuição para planejamento integrado de marketing, auxílio em projetos simultâneos.</t>
+          <t>Mídias de Performance</t>
+        </is>
+      </c>
+      <c r="I16" t="inlineStr">
+        <is>
+          <t>Gestão de mídias pagas, acompanhamento e mensuração de resultados, análises de dados, elaboração de planejamentos, gerenciamento de operações, contribuição para otimização de marketing integrado, auxílio em projetos simultâneos.</t>
         </is>
       </c>
     </row>
@@ -1123,7 +1199,7 @@
       </c>
       <c r="D17" t="inlineStr">
         <is>
-          <t>Cursando Direito a partir do 2° ano, boa comunicação interpessoal, interesse em Legal Tech, Excel Intermediário, boas noções de escrita</t>
+          <t>Cursando Direito a partir do 2° ano, boa comunicação interpessoal, interesse em Legal Tech, Excel intermediário, boas noções de escrita</t>
         </is>
       </c>
       <c r="E17" t="inlineStr">
@@ -1133,17 +1209,22 @@
       </c>
       <c r="F17" t="inlineStr">
         <is>
+          <t>100% Remoto</t>
+        </is>
+      </c>
+      <c r="G17" t="inlineStr">
+        <is>
           <t>Estudantes de Direito</t>
         </is>
       </c>
-      <c r="G17" t="inlineStr">
-        <is>
-          <t>Suporte em tickets relacionados a dúvidas, problemas e tarefas de baixa complexidade</t>
-        </is>
-      </c>
       <c r="H17" t="inlineStr">
         <is>
-          <t>Prestar suporte aos clientes, identificar erros, proporcionar boa experiência aos clientes.</t>
+          <t>Suporte Jurídico</t>
+        </is>
+      </c>
+      <c r="I17" t="inlineStr">
+        <is>
+          <t>Prestar suporte a tickets, identificar erros, proporcionar boa experiência aos clientes</t>
         </is>
       </c>
     </row>
@@ -1165,27 +1246,32 @@
       </c>
       <c r="D18" t="inlineStr">
         <is>
-          <t>Cursando Ensino Superior em Design Gráfico, conhecimento em Figma, noções em desenvolvimento de interfaces, criação de novos produtos e projetos ágeis, inglês avançado/fluente para conversação</t>
+          <t>Cursando Ensino Superior em Design Gráfico, conhecimento em Figma, inglês avançado/fluente</t>
         </is>
       </c>
       <c r="E18" t="inlineStr">
         <is>
-          <t>Salário a combinar</t>
+          <t>A combinar</t>
         </is>
       </c>
       <c r="F18" t="inlineStr">
         <is>
+          <t>Estágio 30h</t>
+        </is>
+      </c>
+      <c r="G18" t="inlineStr">
+        <is>
           <t>Estagiários de Design</t>
         </is>
       </c>
-      <c r="G18" t="inlineStr">
-        <is>
-          <t>UI/UX Design</t>
-        </is>
-      </c>
       <c r="H18" t="inlineStr">
         <is>
-          <t>Criar interfaces e experiências inovadoras, participar de diferentes tipos de projetos, realizar testes de aceitação com o cliente, contribuir para o nível de excelência da equipe de Design, desenvolver interfaces funcionais, entre outras responsabilidades.</t>
+          <t>Design</t>
+        </is>
+      </c>
+      <c r="I18" t="inlineStr">
+        <is>
+          <t>Criar interfaces e experiências inovadoras, participar de testes com usuários, realizar testes de aceitação, desenvolver interfaces funcionais, entre outras.</t>
         </is>
       </c>
     </row>
@@ -1197,7 +1283,7 @@
       </c>
       <c r="B19" t="inlineStr">
         <is>
-          <t>Vendedor Inside Sales</t>
+          <t>Vendedor</t>
         </is>
       </c>
       <c r="C19" t="inlineStr">
@@ -1212,22 +1298,27 @@
       </c>
       <c r="E19" t="inlineStr">
         <is>
-          <t>A combinar</t>
+          <t>Salário a combinar</t>
         </is>
       </c>
       <c r="F19" t="inlineStr">
         <is>
+          <t>Não especificada</t>
+        </is>
+      </c>
+      <c r="G19" t="inlineStr">
+        <is>
           <t>Talentos apaixonados por vendas</t>
         </is>
       </c>
-      <c r="G19" t="inlineStr">
+      <c r="H19" t="inlineStr">
         <is>
           <t>Inside Sales</t>
         </is>
       </c>
-      <c r="H19" t="inlineStr">
-        <is>
-          <t>Conduzir processo comercial, executar sequências de contato, desenvolver relacionamentos com clientes, manter registros de atividades de vendas, observar métricas e indicadores.</t>
+      <c r="I19" t="inlineStr">
+        <is>
+          <t>Conduzir processo comercial, desenvolver relacionamentos com clientes, manter registros de atividades de vendas, observar métricas e indicadores.</t>
         </is>
       </c>
     </row>
@@ -1249,7 +1340,7 @@
       </c>
       <c r="D20" t="inlineStr">
         <is>
-          <t>Cursando Marketing ou Publicidade e Propaganda, conhecimento em ferramentas de marketing digital e design gráfico, habilidades de comunicação, proatividade.</t>
+          <t>Cursando Marketing ou Publicidade e Propaganda, conhecimento em ferramentas de marketing digital e design gráfico, habilidades de comunicação, proatividade</t>
         </is>
       </c>
       <c r="E20" t="inlineStr">
@@ -1259,15 +1350,20 @@
       </c>
       <c r="F20" t="inlineStr">
         <is>
+          <t>6h/dia (segunda-sexta)</t>
+        </is>
+      </c>
+      <c r="G20" t="inlineStr">
+        <is>
           <t>Estudantes de Marketing ou Publicidade e Propaganda</t>
         </is>
       </c>
-      <c r="G20" t="inlineStr">
+      <c r="H20" t="inlineStr">
         <is>
           <t>Marketing, Publicidade e Propaganda</t>
         </is>
       </c>
-      <c r="H20" t="inlineStr">
+      <c r="I20" t="inlineStr">
         <is>
           <t>Criação de materiais gráficos, pesquisa de tendências, desenvolvimento de campanhas, produção de conteúdo, planejamento de mídia, pesquisa de mercado, brainstorming, eventos.</t>
         </is>
@@ -1281,7 +1377,7 @@
       </c>
       <c r="B21" t="inlineStr">
         <is>
-          <t>Estágio de Product Owner</t>
+          <t>Estágio em Engenharia Química</t>
         </is>
       </c>
       <c r="C21" t="inlineStr">
@@ -1291,27 +1387,32 @@
       </c>
       <c r="D21" t="inlineStr">
         <is>
-          <t>Cursando Engenharia, inglês avançado, interesse em ciência de Dados</t>
+          <t>Cursando ensino superior em Engenharia, inglês avançado, interesse em ciência de Dados</t>
         </is>
       </c>
       <c r="E21" t="inlineStr">
         <is>
-          <t>Salário a combinar</t>
+          <t>A combinar</t>
         </is>
       </c>
       <c r="F21" t="inlineStr">
         <is>
-          <t>Estudantes de Engenharia Química com previsão de conclusão para 2026/2</t>
+          <t>30h</t>
         </is>
       </c>
       <c r="G21" t="inlineStr">
         <is>
+          <t>Estudantes de Engenharia</t>
+        </is>
+      </c>
+      <c r="H21" t="inlineStr">
+        <is>
           <t>Desenvolvimento de software para a indústria de Química e Petroquímica</t>
         </is>
       </c>
-      <c r="H21" t="inlineStr">
-        <is>
-          <t>Atuar em projetos de software, discutir e transcrever requisitos, apoiar o time de desenvolvimento, analisar e solucionar problemas.</t>
+      <c r="I21" t="inlineStr">
+        <is>
+          <t>Atuar em projetos de desenvolvimento de software, discutir e transcrever requisitos em inglês, apoiar o time de desenvolvimento, analisar e solucionar problemas.</t>
         </is>
       </c>
     </row>
@@ -1333,7 +1434,7 @@
       </c>
       <c r="D22" t="inlineStr">
         <is>
-          <t>Candidatura simplificada, carreira desafiadora, alta energia, mente aberta</t>
+          <t>Não especificados</t>
         </is>
       </c>
       <c r="E22" t="inlineStr">
@@ -1343,17 +1444,22 @@
       </c>
       <c r="F22" t="inlineStr">
         <is>
+          <t>Não especificada</t>
+        </is>
+      </c>
+      <c r="G22" t="inlineStr">
+        <is>
           <t>Summer Interns e Interns</t>
         </is>
       </c>
-      <c r="G22" t="inlineStr">
-        <is>
-          <t>Estratégia Corporativa e Financeira, Estratégia Digital, Marketing e Vendas, Serviços Transacionais, Operações e Organizações</t>
-        </is>
-      </c>
       <c r="H22" t="inlineStr">
         <is>
-          <t>Compor o time, participar de eventos, adquirir conhecimento.</t>
+          <t>Consultoria de alta gestão</t>
+        </is>
+      </c>
+      <c r="I22" t="inlineStr">
+        <is>
+          <t>Não especificadas</t>
         </is>
       </c>
     </row>
@@ -1375,7 +1481,7 @@
       </c>
       <c r="D23" t="inlineStr">
         <is>
-          <t>Ensino superior, previsão de conclusão, cursos prioritários, postura curiosa e colaborativa, disponibilidade híbrida/presencial</t>
+          <t>Ensino superior, cursos prioritários, perfil colaborativo, disponibilidade híbrida/presencial</t>
         </is>
       </c>
       <c r="E23" t="inlineStr">
@@ -1385,15 +1491,20 @@
       </c>
       <c r="F23" t="inlineStr">
         <is>
-          <t>Estudantes do ensino superior</t>
+          <t>Não especificada</t>
         </is>
       </c>
       <c r="G23" t="inlineStr">
         <is>
+          <t>Estudantes com previsão de conclusão entre dezembro de 2025 a dezembro de 2026</t>
+        </is>
+      </c>
+      <c r="H23" t="inlineStr">
+        <is>
           <t>Engenharias, Administração, Economia, Relações Internacionais, Design, Marketing, Comunicação, Ciências da Computação, Sistemas da Informação, Análise e Desenvolvimento de Sistemas, Matemática, Estatística e áreas afins</t>
         </is>
       </c>
-      <c r="H23" t="inlineStr">
+      <c r="I23" t="inlineStr">
         <is>
           <t>Participar de projetos, elaborar estratégias, trabalhar com tecnologias, atuar em diferentes indústrias e clientes.</t>
         </is>
@@ -1417,7 +1528,7 @@
       </c>
       <c r="D24" t="inlineStr">
         <is>
-          <t>candidatura simplificada, carreira desafiadora</t>
+          <t>Candidatura simplificada, estudantes universitários</t>
         </is>
       </c>
       <c r="E24" t="inlineStr">
@@ -1427,29 +1538,34 @@
       </c>
       <c r="F24" t="inlineStr">
         <is>
+          <t>Não especificada</t>
+        </is>
+      </c>
+      <c r="G24" t="inlineStr">
+        <is>
           <t>Summer Interns e Interns</t>
         </is>
       </c>
-      <c r="G24" t="inlineStr">
+      <c r="H24" t="inlineStr">
         <is>
           <t>Estratégia Corporativa e Financeira, Estratégia Digital, Marketing e Vendas, Serviços Transacionais, Operações e Organizações</t>
         </is>
       </c>
-      <c r="H24" t="inlineStr">
-        <is>
-          <t>Compor o time, participar dos Webinars, realizar provas.</t>
+      <c r="I24" t="inlineStr">
+        <is>
+          <t>Participar do processo seletivo, participar de Webinars, realizar provas.</t>
         </is>
       </c>
     </row>
     <row r="25">
       <c r="A25" t="inlineStr">
         <is>
-          <t>Banco ABC</t>
+          <t>Banco ABC Brasil S/A</t>
         </is>
       </c>
       <c r="B25" t="inlineStr">
         <is>
-          <t>Estagiário(a) em macroeconomia/tesouraria</t>
+          <t>Estagiário(a) na área de macroeconomia/tesouraria</t>
         </is>
       </c>
       <c r="C25" t="inlineStr">
@@ -1459,7 +1575,7 @@
       </c>
       <c r="D25" t="inlineStr">
         <is>
-          <t>Manipulação de dados, conhecimento em métodos quantitativos, cursando graduação em economia, engenharia, matemática ou estatística, inglês avançado</t>
+          <t>Habilidade com manipulação de dados, conhecimento em métodos quantitativos, cursando graduação em economia, engenharia, matemática ou estatística, inglês avançado</t>
         </is>
       </c>
       <c r="E25" t="inlineStr">
@@ -1469,17 +1585,22 @@
       </c>
       <c r="F25" t="inlineStr">
         <is>
-          <t>Estudantes de graduação</t>
+          <t>Horário de estágio a combinar, preferencialmente das 09h às 16h, presencial</t>
         </is>
       </c>
       <c r="G25" t="inlineStr">
         <is>
-          <t>Macroenomia/Tesouraria</t>
+          <t>Estudantes universitários</t>
         </is>
       </c>
       <c r="H25" t="inlineStr">
         <is>
-          <t>Construção e manutenção de base de dados, auxílio em análises para mesas de Trading &amp; ALM, otimização de modelos econômicos, automatização de rotinas.</t>
+          <t>Macroecnomia/Tesouraria</t>
+        </is>
+      </c>
+      <c r="I25" t="inlineStr">
+        <is>
+          <t>Construção e manutenção de base de dados e modelos econométricos, auxílio a análises para as mesas de Trading &amp; ALM, otimização de modelos de projeção econométricos, automatizar rotinas, planilhas e apresentações do departamento econômico e da tesouraria.</t>
         </is>
       </c>
     </row>
@@ -1501,7 +1622,7 @@
       </c>
       <c r="D26" t="inlineStr">
         <is>
-          <t>Cursar Administração, Ciências Econômicas, Engenharias, Ciência de Dados, Matemática ou áreas afins, disponibilidade de 6h/dia por 2 anos, residir em São Paulo/SP, estar conectado aos valores e comportamentos da Eneva</t>
+          <t>Cursar Administração, Ciências Econômicas, Engenharias, Ciência de Dados, Matemática ou áreas afins; disponibilidade de 6h/dia por 2 anos, estar conectado aos valores da empresa, residir em São Paulo/SP</t>
         </is>
       </c>
       <c r="E26" t="inlineStr">
@@ -1511,17 +1632,22 @@
       </c>
       <c r="F26" t="inlineStr">
         <is>
+          <t>6h/dia por 2 anos</t>
+        </is>
+      </c>
+      <c r="G26" t="inlineStr">
+        <is>
           <t>Estudantes universitários</t>
         </is>
       </c>
-      <c r="G26" t="inlineStr">
-        <is>
-          <t>Backoffice, Novos Negócios, Portfólio</t>
-        </is>
-      </c>
       <c r="H26" t="inlineStr">
         <is>
-          <t>Desenvolver habilidades importantes, participar das atividades do dia a dia do negócio, colaborar em um ambiente de trabalho colaborativo e acolhedor.</t>
+          <t>Backoffice, Novos Negócios e Portfólio</t>
+        </is>
+      </c>
+      <c r="I26" t="inlineStr">
+        <is>
+          <t>Desenvolver habilidades e vivenciar o dia a dia do negócio da empresa</t>
         </is>
       </c>
     </row>
@@ -1548,22 +1674,27 @@
       </c>
       <c r="E27" t="inlineStr">
         <is>
-          <t>Salário a combinar</t>
+          <t>A combinar</t>
         </is>
       </c>
       <c r="F27" t="inlineStr">
         <is>
-          <t>Estagiários de Psicologia ou áreas afins</t>
+          <t>6hs diárias</t>
         </is>
       </c>
       <c r="G27" t="inlineStr">
         <is>
-          <t>Business Partner</t>
+          <t>Estudantes de Psicologia ou áreas afins</t>
         </is>
       </c>
       <c r="H27" t="inlineStr">
         <is>
-          <t>Apoio no Onboarding de estagiários/staff, suporte em relatórios, cadastro de informações e atualizações da área, acompanhamento e cobranças de pendências, atendimento e suporte aos clientes internos.</t>
+          <t>Business Partner, Consultoria Tributária</t>
+        </is>
+      </c>
+      <c r="I27" t="inlineStr">
+        <is>
+          <t>Apoio no Onboarding, suporte em relatórios, cadastro de informações, acompanhamento de pendências, atendimento aos clientes internos</t>
         </is>
       </c>
     </row>
@@ -1575,7 +1706,7 @@
       </c>
       <c r="B28" t="inlineStr">
         <is>
-          <t>Estágio em Controle de Qualidade</t>
+          <t>Controle de Qualidade</t>
         </is>
       </c>
       <c r="C28" t="inlineStr">
@@ -1585,7 +1716,7 @@
       </c>
       <c r="D28" t="inlineStr">
         <is>
-          <t>Cursando superior em Engenharia (Mecânica, Elétrica, Química, Produção ou Metalúrgica), Inglês avançado, Conhecimento em Pacote office (principalmente excel e PPT)</t>
+          <t>Cursando superior em Engenharia, Inglês avançado, Conhecimento em Pacote Office</t>
         </is>
       </c>
       <c r="E28" t="inlineStr">
@@ -1595,17 +1726,22 @@
       </c>
       <c r="F28" t="inlineStr">
         <is>
+          <t>Flexível</t>
+        </is>
+      </c>
+      <c r="G28" t="inlineStr">
+        <is>
           <t>Estudantes de Engenharia</t>
         </is>
       </c>
-      <c r="G28" t="inlineStr">
+      <c r="H28" t="inlineStr">
         <is>
           <t>Controle de Qualidade</t>
         </is>
       </c>
-      <c r="H28" t="inlineStr">
-        <is>
-          <t>Auxiliar os analistas da área na interface entre o fornecedor e a fábrica de Manaus, Follow ups das ocorrências, Auxiliar na elaboração de relatórios de amostras, Auxiliar na emissão de controle de lote inicial.</t>
+      <c r="I28" t="inlineStr">
+        <is>
+          <t>Auxiliar os analistas da área, Follow ups das ocorrências, Elaboração de relatórios, Emissão de controle de lote.</t>
         </is>
       </c>
     </row>
@@ -1627,27 +1763,32 @@
       </c>
       <c r="D29" t="inlineStr">
         <is>
-          <t>Cursar Administração, Ciências Econômicas, Engenharias, Ciência de Dados, Matemática ou áreas afins, disponibilidade de 6h/dia por 2 anos, residir em São Paulo/SP, estar conectado aos valores e comportamentos da Eneva</t>
+          <t>Cursar Administração, Ciências Econômicas, Engenharias, Ciência de Dados, Matemática ou áreas afins; disponibilidade de 6h/dia por 2 anos; residir em São Paulo/SP</t>
         </is>
       </c>
       <c r="E29" t="inlineStr">
         <is>
-          <t>Bolsa auxílio</t>
+          <t>Salário a combinar, bolsa auxílio</t>
         </is>
       </c>
       <c r="F29" t="inlineStr">
         <is>
+          <t>6h/dia</t>
+        </is>
+      </c>
+      <c r="G29" t="inlineStr">
+        <is>
           <t>Estudantes universitários</t>
         </is>
       </c>
-      <c r="G29" t="inlineStr">
-        <is>
-          <t>Backoffice, Novos Negócios e Portfólio</t>
-        </is>
-      </c>
       <c r="H29" t="inlineStr">
         <is>
-          <t>Desenvolver habilidades práticas, vivenciar o dia a dia do negócio da empresa, participar do programa de desenvolvimento e mentoria.</t>
+          <t>Backoffice, Novos Negócios, Portfólio</t>
+        </is>
+      </c>
+      <c r="I29" t="inlineStr">
+        <is>
+          <t>Desenvolver habilidades e vivenciar o dia a dia do negócio, participar do programa de desenvolvimento e mentoria</t>
         </is>
       </c>
     </row>
@@ -1669,7 +1810,7 @@
       </c>
       <c r="D30" t="inlineStr">
         <is>
-          <t>Experiência em funções administrativas ou financeiras, conhecimento em software de contabilidade SAP 4/Hana, formação em Administração, Gestão Financeira, Contabilidade ou área relacionada</t>
+          <t>Experiência em contas a pagar, capacidade analítica, formação em Administração ou áreas relacionadas</t>
         </is>
       </c>
       <c r="E30" t="inlineStr">
@@ -1679,17 +1820,22 @@
       </c>
       <c r="F30" t="inlineStr">
         <is>
-          <t>Pessoas organizadas, inovadoras, resilientes e com forte senso de responsabilidade</t>
+          <t>Não especificada</t>
         </is>
       </c>
       <c r="G30" t="inlineStr">
         <is>
-          <t>Financeira</t>
+          <t>Não especificado</t>
         </is>
       </c>
       <c r="H30" t="inlineStr">
         <is>
-          <t>Processamento de pagamentos, revisão de faturas, conciliações bancárias, relacionamento com fornecedores, organização de documentos, colaboração em auditorias, cumprimento de políticas financeiras e requisitos legais.</t>
+          <t>Financeiro</t>
+        </is>
+      </c>
+      <c r="I30" t="inlineStr">
+        <is>
+          <t>Processar pagamentos, revisar faturas, conciliar extratos bancários, manter arquivos organizados.</t>
         </is>
       </c>
     </row>
@@ -1711,7 +1857,7 @@
       </c>
       <c r="D31" t="inlineStr">
         <is>
-          <t>Estudantes de Negócios, Economia, Contabilidade, Engenharia ou áreas relacionadas, turno noturno, formatura em 1,5 anos ou mais, inglês fluente</t>
+          <t>Students of Business, Economics, Accounting, Engineering or related courses, Night shift students, Expecting to graduate in 1.5 year or more, Fluent English is mandatory</t>
         </is>
       </c>
       <c r="E31" t="inlineStr">
@@ -1721,17 +1867,22 @@
       </c>
       <c r="F31" t="inlineStr">
         <is>
-          <t>Estudantes de graduação</t>
+          <t>Não especificada</t>
         </is>
       </c>
       <c r="G31" t="inlineStr">
         <is>
+          <t>Estudantes de cursos relacionados</t>
+        </is>
+      </c>
+      <c r="H31" t="inlineStr">
+        <is>
           <t>Corporate Banking</t>
         </is>
       </c>
-      <c r="H31" t="inlineStr">
-        <is>
-          <t>Prover uma ampla gama de produtos relacionados a empréstimos e serviços financeiros para grandes empresas globais, construir relacionamentos de longo prazo com grandes corporações e instituições financeiras multinacionais, fornecer produtos e serviços relacionados às atividades de empréstimo entre um banco e seus clientes.</t>
+      <c r="I31" t="inlineStr">
+        <is>
+          <t>Fornecer uma ampla gama de produtos relacionados a empréstimos e serviços financeiros para grandes empresas. Construir relacionamentos de longo prazo com grandes corporações e instituições financeiras. Fornecer produtos e serviços relacionados às atividades de empréstimo entre um banco e seus clientes.</t>
         </is>
       </c>
     </row>
@@ -1753,7 +1904,7 @@
       </c>
       <c r="D32" t="inlineStr">
         <is>
-          <t>Graduação em Administração, Tecnologia, Engenharias e/ou correlatas; Conhecimento básico em SQL, Phyton, PySpark e Power Querry (diferencial)</t>
+          <t>Graduação em Administração, Tecnologia, Engenharias e/ou correlatas. Conhecimento básico em SQL, Phyton, PySpark e Power Query (diferencial).</t>
         </is>
       </c>
       <c r="E32" t="inlineStr">
@@ -1763,17 +1914,22 @@
       </c>
       <c r="F32" t="inlineStr">
         <is>
-          <t>Todas as nossas vagas estão abertas para Pessoas com Deficiência (PCDs)</t>
+          <t>Não especificada</t>
         </is>
       </c>
       <c r="G32" t="inlineStr">
         <is>
-          <t>Qualidade</t>
+          <t>Todas as vagas abertas para Pessoas com Deficiência (PCDs)</t>
         </is>
       </c>
       <c r="H32" t="inlineStr">
         <is>
-          <t>Auxiliar na apuração e construção de Dashboard em Power BI; Auxiliar na criação de novas pesquisas (SQL, Phyton e PySpark); Auxiliar no mapeamento da experiência do cliente.</t>
+          <t>Qualidade, Analytics e Dados</t>
+        </is>
+      </c>
+      <c r="I32" t="inlineStr">
+        <is>
+          <t>Auxiliar na apuração e construção de Dashboard em Power BI, auxiliar na criação de novas pesquisas (SQL, Phyton e PySpark), auxiliar no mapeamento da experiência do cliente.</t>
         </is>
       </c>
     </row>
@@ -1785,7 +1941,7 @@
       </c>
       <c r="B33" t="inlineStr">
         <is>
-          <t>Banco de Talentos Afirmativo para Pessoas com Deficiência (PCD) - Comercial</t>
+          <t>Comercial</t>
         </is>
       </c>
       <c r="C33" t="inlineStr">
@@ -1795,7 +1951,7 @@
       </c>
       <c r="D33" t="inlineStr">
         <is>
-          <t>Pessoa com deficiência com CID homologado</t>
+          <t>Pessoas com deficiência com CID homologado</t>
         </is>
       </c>
       <c r="E33" t="inlineStr">
@@ -1805,17 +1961,22 @@
       </c>
       <c r="F33" t="inlineStr">
         <is>
+          <t>Não especificada</t>
+        </is>
+      </c>
+      <c r="G33" t="inlineStr">
+        <is>
           <t>Pessoas com deficiência com CID homologado</t>
         </is>
       </c>
-      <c r="G33" t="inlineStr">
+      <c r="H33" t="inlineStr">
         <is>
           <t>Comercial</t>
         </is>
       </c>
-      <c r="H33" t="inlineStr">
-        <is>
-          <t>Trabalhar com a equipe do Agibank, passar por triagem, ser redirecionado para vagas compatíveis, participar das etapas de seleção.</t>
+      <c r="I33" t="inlineStr">
+        <is>
+          <t>Não especificadas</t>
         </is>
       </c>
     </row>
@@ -1837,7 +1998,7 @@
       </c>
       <c r="D34" t="inlineStr">
         <is>
-          <t>Strong academic background, analytical skills, high motivation levels, outstanding interpersonal skills</t>
+          <t>Strong academic background, analytical skills, high motivation levels, outstanding interpersonal skills, on track to graduate by June 2026</t>
         </is>
       </c>
       <c r="E34" t="inlineStr">
@@ -1847,17 +2008,22 @@
       </c>
       <c r="F34" t="inlineStr">
         <is>
-          <t>Estudantes atuais</t>
+          <t>Não especificada</t>
         </is>
       </c>
       <c r="G34" t="inlineStr">
         <is>
-          <t>Consultoria</t>
+          <t>Current students</t>
         </is>
       </c>
       <c r="H34" t="inlineStr">
         <is>
-          <t>Trabalhar em equipe, entrevistar clientes, identificar fontes de informação, apresentar resultados</t>
+          <t>Consulting industry, business strategy</t>
+        </is>
+      </c>
+      <c r="I34" t="inlineStr">
+        <is>
+          <t>Work on a case team, interview clients' customers, competitors, suppliers and employers, own and identify information sources, gather and interpret data, execute analysis, present findings to case team members and client stakeholders.</t>
         </is>
       </c>
     </row>
@@ -1879,7 +2045,7 @@
       </c>
       <c r="D35" t="inlineStr">
         <is>
-          <t>Experiência com Customer Success, retenção de clientes, habilidades de comunicação, formação em Marketing, Comunicação ou Administração</t>
+          <t>Experiência com Customer Success, retenção de clientes, comunicação verbal e escrita, habilidades analíticas</t>
         </is>
       </c>
       <c r="E35" t="inlineStr">
@@ -1889,17 +2055,22 @@
       </c>
       <c r="F35" t="inlineStr">
         <is>
+          <t>Não especificada</t>
+        </is>
+      </c>
+      <c r="G35" t="inlineStr">
+        <is>
           <t>Profissionais motivados, orientados para resultados, apaixonados por ajudar os clientes</t>
         </is>
       </c>
-      <c r="G35" t="inlineStr">
-        <is>
-          <t>Customer Success, Customer Experience</t>
-        </is>
-      </c>
       <c r="H35" t="inlineStr">
         <is>
-          <t>Desenvolver e manter relacionamentos com clientes, entender metas dos clientes, resolver problemas, colaborar com equipes internas, gerenciar reclamações, fidelizar clientes</t>
+          <t>Customer Success, Customer Experience, Marketing Digital</t>
+        </is>
+      </c>
+      <c r="I35" t="inlineStr">
+        <is>
+          <t>Desenvolver e manter relacionamentos com clientes, entender metas e objetivos dos clientes, resolver problemas dos clientes, colaborar com equipes internas, promover a melhor experiência aos clientes, gerenciar reclamações, diminuir taxas de churn.</t>
         </is>
       </c>
     </row>
@@ -1921,7 +2092,7 @@
       </c>
       <c r="D36" t="inlineStr">
         <is>
-          <t>Experiência em lidar com clientes, formação em áreas relacionadas ao treinamento, habilidades de comunicação, capacidade de se adaptar a mudanças</t>
+          <t>Experiência prévia em lidar com clientes, habilidades de comunicação, capacidade de se adaptar a mudanças</t>
         </is>
       </c>
       <c r="E36" t="inlineStr">
@@ -1931,17 +2102,22 @@
       </c>
       <c r="F36" t="inlineStr">
         <is>
+          <t>Não especificada</t>
+        </is>
+      </c>
+      <c r="G36" t="inlineStr">
+        <is>
           <t>Não especificado</t>
         </is>
       </c>
-      <c r="G36" t="inlineStr">
-        <is>
-          <t>Educação</t>
-        </is>
-      </c>
       <c r="H36" t="inlineStr">
         <is>
-          <t>Prestar suporte aos clientes, propor soluções de desenvolvimento, atualizar e analisar indicadores, organizar operacionalização das turmas.</t>
+          <t>Treinamento e Desenvolvimento</t>
+        </is>
+      </c>
+      <c r="I36" t="inlineStr">
+        <is>
+          <t>Prestar suporte para os clientes, propor soluções de desenvolvimento, atualizar e analisar indicadores, organizar operacionalização das turmas.</t>
         </is>
       </c>
     </row>
@@ -1963,7 +2139,7 @@
       </c>
       <c r="D37" t="inlineStr">
         <is>
-          <t>habilidades analíticas, capacidade de influenciar entregas de projetos</t>
+          <t>desenvolvimento de habilidades analíticas</t>
         </is>
       </c>
       <c r="E37" t="inlineStr">
@@ -1973,17 +2149,22 @@
       </c>
       <c r="F37" t="inlineStr">
         <is>
-          <t>Estudantes em busca de desenvolvimento pessoal</t>
+          <t>Não especificada</t>
         </is>
       </c>
       <c r="G37" t="inlineStr">
         <is>
+          <t>Estudantes interessados na carreira de consultor</t>
+        </is>
+      </c>
+      <c r="H37" t="inlineStr">
+        <is>
           <t>Consultoria estratégica</t>
         </is>
       </c>
-      <c r="H37" t="inlineStr">
-        <is>
-          <t>Desenvolvimento de habilidades analíticas, participação em projetos de consultoria, aprendizado nas 4 dimensões da Mirow.</t>
+      <c r="I37" t="inlineStr">
+        <is>
+          <t>Influenciar as entregas dos projetos, desenvolver habilidades analíticas</t>
         </is>
       </c>
     </row>
@@ -2005,7 +2186,7 @@
       </c>
       <c r="D38" t="inlineStr">
         <is>
-          <t>Cursando Administração, Ciências Contábeis, Engenharia da Produção; Conhecimento em Pacote Office; Desejável conhecimento em Google Workspace e SAP</t>
+          <t>Cursando Administração, Ciências Contábeis, Engenharia da Produção; Conhecimento em Pacote Office, Excel e desejável Google Workspace e SAP; Habilidades em organização, comunicação, análise, atenção aos detalhes e proatividade</t>
         </is>
       </c>
       <c r="E38" t="inlineStr">
@@ -2015,17 +2196,22 @@
       </c>
       <c r="F38" t="inlineStr">
         <is>
-          <t>Estudantes de Ensino Superior com formação prevista após Julho de 2025</t>
+          <t>6 horas diárias, segunda a sexta</t>
         </is>
       </c>
       <c r="G38" t="inlineStr">
         <is>
-          <t>Administração, Finanças</t>
+          <t>Estudantes matriculados em Instituição de Ensino Superior, formação após julho de 2025, residir em São Paulo com fácil acesso à região da Vila Olímpia</t>
         </is>
       </c>
       <c r="H38" t="inlineStr">
         <is>
-          <t>Auxiliar em rotinas administrativas e financeiras, controle de pagamento, conferência de dados financeiros, análise de desempenho financeiro dos contratos, cumprimento dos fluxos de procedimentos administrativos e financeiros, suporte nas atividades da área.</t>
+          <t>Administrativo e Financeiro</t>
+        </is>
+      </c>
+      <c r="I38" t="inlineStr">
+        <is>
+          <t>Auxiliar em rotinas administrativas e financeiras, controle de pagamentos, conferência de dados financeiros, análise de desempenho financeiro dos contratos, cumprimento dos fluxos de procedimentos administrativos e financeiros, suporte nas atividades da área.</t>
         </is>
       </c>
     </row>
@@ -2047,7 +2233,7 @@
       </c>
       <c r="D39" t="inlineStr">
         <is>
-          <t>Cursando Ensino Superior, interesse em mercado financeiro, conhecimento em Pacote Office, inglês básico</t>
+          <t>Cursando Ensino Superior, Interesse por mercado financeiro, Conhecimento intermediário em Pacote Office, Inglês básico</t>
         </is>
       </c>
       <c r="E39" t="inlineStr">
@@ -2057,17 +2243,22 @@
       </c>
       <c r="F39" t="inlineStr">
         <is>
+          <t>Híbrido (1 a 3 vezes na semana no escritório)</t>
+        </is>
+      </c>
+      <c r="G39" t="inlineStr">
+        <is>
           <t>Estudantes de Direito, Ciências Econômicas, Contabilidade, entre outros</t>
         </is>
       </c>
-      <c r="G39" t="inlineStr">
-        <is>
-          <t>DCM (Estruturação, originação, distribuição de CRI, CRA, FIDC, FIAgros, Debêntures)</t>
-        </is>
-      </c>
       <c r="H39" t="inlineStr">
         <is>
-          <t>Suporte ao time de DCM, participação em calls, uso de ferramentas do time, habilidades de resolução de problemas, comunicação, trabalho em equipe, análise crítica, flexibilidade, organização, atenção aos detalhes.</t>
+          <t>DCM (Estruturação)</t>
+        </is>
+      </c>
+      <c r="I39" t="inlineStr">
+        <is>
+          <t>Suporte operacional e administrativo, Participação no processo de originação, estruturação e distribuição, Uso de ferramentas do time de DCM, Habilidade de resolver problemas, Capacidade de comunicação e trabalho em equipe, Análise crítica, Flexibilidade, Organização e atenção aos detalhes.</t>
         </is>
       </c>
     </row>
@@ -2089,7 +2280,7 @@
       </c>
       <c r="D40" t="inlineStr">
         <is>
-          <t>18 anos, matrícula ativa em universidade, disponibilidade de 15h semanais, interesse em vendas e trabalho voluntário</t>
+          <t>18 anos, matrícula ativa em universidade, disponibilidade de 15h semanais, interesse por vendas e trabalho voluntário</t>
         </is>
       </c>
       <c r="E40" t="inlineStr">
@@ -2099,15 +2290,20 @@
       </c>
       <c r="F40" t="inlineStr">
         <is>
+          <t>5 semanas, 15h semanais</t>
+        </is>
+      </c>
+      <c r="G40" t="inlineStr">
+        <is>
           <t>Estudantes universitários</t>
         </is>
       </c>
-      <c r="G40" t="inlineStr">
+      <c r="H40" t="inlineStr">
         <is>
           <t>Vendas, operações, divulgação</t>
         </is>
       </c>
-      <c r="H40" t="inlineStr">
+      <c r="I40" t="inlineStr">
         <is>
           <t>Vendas, operações, divulgação</t>
         </is>
@@ -2131,7 +2327,7 @@
       </c>
       <c r="D41" t="inlineStr">
         <is>
-          <t>Experiência em cobrança ou atendimento ao cliente, habilidades de comunicação, formação em Administração, Gestão Financeira ou Contabilidade</t>
+          <t>Experiência em cobrança, habilidades de comunicação, formação em Administração ou áreas relacionadas</t>
         </is>
       </c>
       <c r="E41" t="inlineStr">
@@ -2141,17 +2337,22 @@
       </c>
       <c r="F41" t="inlineStr">
         <is>
+          <t>Não especificada</t>
+        </is>
+      </c>
+      <c r="G41" t="inlineStr">
+        <is>
           <t>Não especificado</t>
         </is>
       </c>
-      <c r="G41" t="inlineStr">
-        <is>
-          <t>Financeiro</t>
-        </is>
-      </c>
       <c r="H41" t="inlineStr">
         <is>
-          <t>Contato com clientes inadimplentes, negociação de pagamento, controle de faturamentos, emissão de boletos e notas fiscais</t>
+          <t>Financeira</t>
+        </is>
+      </c>
+      <c r="I41" t="inlineStr">
+        <is>
+          <t>Contato com clientes inadimplentes, negociação de pagamentos, controle de faturamento, emissão de boletos e notas fiscais</t>
         </is>
       </c>
     </row>
@@ -2163,7 +2364,7 @@
       </c>
       <c r="B42" t="inlineStr">
         <is>
-          <t>ACI - Associate Consultant Intern (estágio regular - 6 a 12 meses)</t>
+          <t>AC - Associate Consultant Intern (estágio regular - 6 a 12 meses)</t>
         </is>
       </c>
       <c r="C42" t="inlineStr">
@@ -2173,7 +2374,7 @@
       </c>
       <c r="D42" t="inlineStr">
         <is>
-          <t>Estudante universitário ou recém formado</t>
+          <t>Estudante universitário (ou recém formado)</t>
         </is>
       </c>
       <c r="E42" t="inlineStr">
@@ -2183,17 +2384,22 @@
       </c>
       <c r="F42" t="inlineStr">
         <is>
-          <t>Estudantes universitários ou recém formados</t>
+          <t>Não especificada</t>
         </is>
       </c>
       <c r="G42" t="inlineStr">
         <is>
+          <t>Estudantes universitários (ou recém formados)</t>
+        </is>
+      </c>
+      <c r="H42" t="inlineStr">
+        <is>
           <t>Consultoria estratégica</t>
         </is>
       </c>
-      <c r="H42" t="inlineStr">
-        <is>
-          <t>Trabalhar em equipe, coletar e interpretar dados, entrevistar stakeholders, supervisionar colegas.</t>
+      <c r="I42" t="inlineStr">
+        <is>
+          <t>Identificação de fontes de informação, coleta e interpretação de dados, execução de análises, apresentação de resultados, entrevistas com consumidores, supervisão de colegas.</t>
         </is>
       </c>
     </row>
@@ -2215,7 +2421,7 @@
       </c>
       <c r="D43" t="inlineStr">
         <is>
-          <t>Ensino Superior em andamento, Boas habilidades com o Pacote Office, Disponibilidade para atuar em formato de trabalho híbrido em Porto Alegre/RS, Proatividade, comunicação, flexibilidade, organização e bom relacionamento interpessoal</t>
+          <t>Ensino Superior em andamento, Pacote Office, disponibilidade para trabalho híbrido em Porto Alegre/RS, proatividade, comunicação, flexibilidade, organização, bom relacionamento interpessoal</t>
         </is>
       </c>
       <c r="E43" t="inlineStr">
@@ -2225,17 +2431,22 @@
       </c>
       <c r="F43" t="inlineStr">
         <is>
+          <t>Não especificada</t>
+        </is>
+      </c>
+      <c r="G43" t="inlineStr">
+        <is>
           <t>Estudantes de Ensino Superior</t>
         </is>
       </c>
-      <c r="G43" t="inlineStr">
-        <is>
-          <t>Recursos Humanos, Desenvolvimento, Talent Acquisition</t>
-        </is>
-      </c>
       <c r="H43" t="inlineStr">
         <is>
-          <t>Encontrar, qualificar e nutrir relacionamento com talentos, mapear talentos no mercado, realizar entrevistas por competências, apoiar no processo de admissão de novos colaboradores, gerir plataformas de seleção.</t>
+          <t>Recursos Humanos, Desenvolvimento, Atração e Seleção</t>
+        </is>
+      </c>
+      <c r="I43" t="inlineStr">
+        <is>
+          <t>Encontrar, qualificar e nutrir relacionamento com talentos, mapear talentos, realizar entrevistas, auxiliar no processo de admissão, gerir plataformas de seleção.</t>
         </is>
       </c>
     </row>
@@ -2257,7 +2468,7 @@
       </c>
       <c r="D44" t="inlineStr">
         <is>
-          <t>Graduação em andamento em Ciências Agrárias, disponibilidade eventual de estar presente no laboratório</t>
+          <t>Graduação em Ciências Agrárias, conhecimento na área de interesse, disponibilidade para estar presente nas unidades de MG ou SP</t>
         </is>
       </c>
       <c r="E44" t="inlineStr">
@@ -2267,17 +2478,22 @@
       </c>
       <c r="F44" t="inlineStr">
         <is>
+          <t>Não especificada</t>
+        </is>
+      </c>
+      <c r="G44" t="inlineStr">
+        <is>
           <t>Estudantes dos cursos de Ciências Agrárias</t>
         </is>
       </c>
-      <c r="G44" t="inlineStr">
+      <c r="H44" t="inlineStr">
         <is>
           <t>Comercial, Vendas Internas</t>
         </is>
       </c>
-      <c r="H44" t="inlineStr">
-        <is>
-          <t>Dar apoio nos processos de vendas internas, aprender sobre produtos e serviços, entender necessidades dos clientes.</t>
+      <c r="I44" t="inlineStr">
+        <is>
+          <t>Apoio nos processos de vendas internas, contato direto com clientes, acompanhamento de pedidos, suporte ao pós-venda, aprendizado sobre produtos e serviços, entendimento das necessidades dos clientes.</t>
         </is>
       </c>
     </row>
@@ -2299,7 +2515,7 @@
       </c>
       <c r="D45" t="inlineStr">
         <is>
-          <t>Ciência da Computação, Engenharias, Sistemas de Informação, conhecimento básico em metodologias ágeis, padrões de projeto e arquitetura de sistemas, conhecimento básico em pelo menos uma linguagem de programação e framework</t>
+          <t>Ciência da Computação, Engenharias, Sistemas de Informação, conhecimento básico em metodologias ágeis, linguagem de programação e framework</t>
         </is>
       </c>
       <c r="E45" t="inlineStr">
@@ -2309,17 +2525,22 @@
       </c>
       <c r="F45" t="inlineStr">
         <is>
+          <t>Não especificada</t>
+        </is>
+      </c>
+      <c r="G45" t="inlineStr">
+        <is>
           <t>Universitários</t>
         </is>
       </c>
-      <c r="G45" t="inlineStr">
+      <c r="H45" t="inlineStr">
         <is>
           <t>Engenharia de Dados, Automação de Processos, Gestão de TI, Desenvolvimento de Software</t>
         </is>
       </c>
-      <c r="H45" t="inlineStr">
-        <is>
-          <t>Desenvolvimento front-end e/ou back-end, correção de bugs, definição de tecnologias, implementação de ferramentas, compartilhar conhecimento.</t>
+      <c r="I45" t="inlineStr">
+        <is>
+          <t>Desenvolvimento front-end e/ou back-end, correção de bugs, definição de tecnologias, implementação de novas ferramentas</t>
         </is>
       </c>
     </row>
@@ -2331,7 +2552,7 @@
       </c>
       <c r="B46" t="inlineStr">
         <is>
-          <t>Estágio</t>
+          <t>Programa de Estágio</t>
         </is>
       </c>
       <c r="C46" t="inlineStr">
@@ -2341,7 +2562,7 @@
       </c>
       <c r="D46" t="inlineStr">
         <is>
-          <t>Graduação a partir do 6º período, Conhecimento em alguma linguagem de programação, Inglês avançado</t>
+          <t>Graduação a partir do 6º período, conhecimento em linguagem de programação, inglês avançado</t>
         </is>
       </c>
       <c r="E46" t="inlineStr">
@@ -2351,17 +2572,22 @@
       </c>
       <c r="F46" t="inlineStr">
         <is>
+          <t>Não especificada</t>
+        </is>
+      </c>
+      <c r="G46" t="inlineStr">
+        <is>
           <t>Estudantes universitários</t>
         </is>
       </c>
-      <c r="G46" t="inlineStr">
-        <is>
-          <t>Tecnologia, RPA, Business Analytics</t>
-        </is>
-      </c>
       <c r="H46" t="inlineStr">
         <is>
-          <t>Contribuir para entrega de soluções de automação, Desenvolver soluções em RPA</t>
+          <t>Tech, RPA (Robotic Process Automation), Business Analytics</t>
+        </is>
+      </c>
+      <c r="I46" t="inlineStr">
+        <is>
+          <t>Contribuir para entrega de soluções de automação, desenvolver soluções em RPA</t>
         </is>
       </c>
     </row>
@@ -2383,7 +2609,7 @@
       </c>
       <c r="D47" t="inlineStr">
         <is>
-          <t>Cursando engenharia, inglês avançado, excel intermediário/avançado, capacidade de gerenciamento de tempo e resolução de problemas, vontade de aprender e se desenvolver</t>
+          <t>Cursando Engenharia de Processos, Mecânica, Automação ou áreas correlatas, Inglês Avançado/Fluente, Excel Intermediário/Avançado, Capacidade de gerenciamento de tempo e resolução de problemas, Vontade de aprender e se desenvolver</t>
         </is>
       </c>
       <c r="E47" t="inlineStr">
@@ -2393,17 +2619,22 @@
       </c>
       <c r="F47" t="inlineStr">
         <is>
-          <t>Estudantes de engenharia e áreas correlatas com formação prevista para a partir de 2025/2</t>
+          <t>Estágio 30h</t>
         </is>
       </c>
       <c r="G47" t="inlineStr">
         <is>
+          <t>Estudantes com formação prevista para a partir de 2025/2</t>
+        </is>
+      </c>
+      <c r="H47" t="inlineStr">
+        <is>
           <t>Desenvolvimento de Negócios</t>
         </is>
       </c>
-      <c r="H47" t="inlineStr">
-        <is>
-          <t>Mapeamento e prospecção de oportunidades, pesquisas de mercado, elaboração de propostas, acompanhamento de equipe técnica, representação da empresa em reuniões, apoio na construção de propostas comerciais, elaboração de materiais de divulgação.</t>
+      <c r="I47" t="inlineStr">
+        <is>
+          <t>Mapeamento e prospecção de oportunidades, Realizar pesquisas de mercado, Elaborar propostas técnicas-comerciais, Acompanhar equipe técnica, Representar a empresa em reuniões, Elaborar materiais de divulgação.</t>
         </is>
       </c>
     </row>
@@ -2425,7 +2656,7 @@
       </c>
       <c r="D48" t="inlineStr">
         <is>
-          <t>Formatura a partir de Dez/25, capacidade analítica e criativa, proatividade, boa comunicação, Excel &amp; PowerPoint avançado, Inglês avançado, SQL e Python são diferenciais</t>
+          <t>Formatura a partir de Dez/25, capacidade analítica, pro atividade, boa comunicação, Excel &amp; PowerPoint avançado, Inglês avançado, SQL e Python são diferenciais</t>
         </is>
       </c>
       <c r="E48" t="inlineStr">
@@ -2435,15 +2666,20 @@
       </c>
       <c r="F48" t="inlineStr">
         <is>
-          <t>Pessoas sem distinção</t>
+          <t>Não especificada</t>
         </is>
       </c>
       <c r="G48" t="inlineStr">
         <is>
-          <t>Business Intelligence</t>
+          <t>Formandos a partir de Dez/25</t>
         </is>
       </c>
       <c r="H48" t="inlineStr">
+        <is>
+          <t>Growth - Business Intelligence</t>
+        </is>
+      </c>
+      <c r="I48" t="inlineStr">
         <is>
           <t>Elaborar modelos de projeção de receita e custos, elaborar modelos de projeção por canais de marketing, auxiliar na resolução de problemas, acompanhar a performance de testes de Growth, automatizar processos recorrentes, explicar resultados e alinhar planos de ação, elaborar apresentações.</t>
         </is>

</xml_diff>